<commit_message>
V02 list 修改 20221228-001
</commit_message>
<xml_diff>
--- a/list_V02 - 副本4.xlsx
+++ b/list_V02 - 副本4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zz\PycharmProjects\IQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7841F163-4C04-420C-BD3C-A7BF3462BB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B97095-FDD7-4981-965E-225DCA6AADA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="6828" windowWidth="23256" windowHeight="12576" tabRatio="458" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11413" uniqueCount="1966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11422" uniqueCount="1966">
   <si>
     <t>物料号</t>
   </si>
@@ -7371,8 +7371,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:BP324"/>
   <sheetViews>
-    <sheetView topLeftCell="AL1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="W1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AM1" sqref="AM1"/>
     </sheetView>
   </sheetViews>
@@ -7652,7 +7652,7 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="2" spans="1:68" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:68" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>275</v>
       </c>
@@ -7819,7 +7819,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:68" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:68" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>276</v>
       </c>
@@ -7986,7 +7986,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:68" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:68" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>241</v>
       </c>
@@ -8153,7 +8153,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:68" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:68" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>243</v>
       </c>
@@ -8320,7 +8320,7 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="6" spans="1:68" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:68" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>262</v>
       </c>
@@ -8469,7 +8469,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:68" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:68" ht="28.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B7" s="8">
         <v>7</v>
       </c>
@@ -8633,7 +8633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:68" s="12" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:68" s="12" customFormat="1" ht="28.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>273</v>
       </c>
@@ -8800,7 +8800,7 @@
         <v>1952</v>
       </c>
     </row>
-    <row r="9" spans="1:68" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:68" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>260</v>
       </c>
@@ -8967,7 +8967,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:68" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:68" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>259</v>
       </c>
@@ -9116,7 +9116,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:68" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:68" ht="28.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>263</v>
       </c>
@@ -9265,7 +9265,7 @@
         <v>1952</v>
       </c>
     </row>
-    <row r="12" spans="1:68" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:68" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>236</v>
       </c>
@@ -31110,7 +31110,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="180" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="5">
         <v>271</v>
       </c>
@@ -31277,7 +31277,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="181" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="5">
         <v>272</v>
       </c>
@@ -31444,7 +31444,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="182" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="5">
         <v>277</v>
       </c>
@@ -31611,7 +31611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="183" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="5">
         <v>261</v>
       </c>
@@ -31775,7 +31775,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="184" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="5">
         <v>280</v>
       </c>
@@ -31942,7 +31942,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="185" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="5">
         <v>281</v>
       </c>
@@ -32091,7 +32091,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="186" spans="1:55" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:55" ht="28.5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="5">
         <v>279</v>
       </c>
@@ -32240,7 +32240,7 @@
         <v>1952</v>
       </c>
     </row>
-    <row r="187" spans="1:55" ht="57" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:55" ht="57" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="5">
         <v>278</v>
       </c>
@@ -32407,7 +32407,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="188" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="5">
         <v>268</v>
       </c>
@@ -32574,7 +32574,7 @@
         <v>1553</v>
       </c>
     </row>
-    <row r="189" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="5">
         <v>269</v>
       </c>
@@ -32741,7 +32741,7 @@
         <v>1553</v>
       </c>
     </row>
-    <row r="190" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="5">
         <v>282</v>
       </c>
@@ -32908,7 +32908,7 @@
         <v>1553</v>
       </c>
     </row>
-    <row r="191" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="5">
         <v>283</v>
       </c>
@@ -33057,7 +33057,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="192" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="5">
         <v>270</v>
       </c>
@@ -33188,7 +33188,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="193" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="5">
         <v>267</v>
       </c>
@@ -33355,7 +33355,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:55" ht="57" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:55" ht="57" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="5">
         <v>289</v>
       </c>
@@ -33522,7 +33522,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="195" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="5">
         <v>246</v>
       </c>
@@ -33689,7 +33689,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="196" spans="1:55" ht="57" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:55" ht="57" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="5">
         <v>314</v>
       </c>
@@ -33856,7 +33856,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="197" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="5">
         <v>356</v>
       </c>
@@ -34005,7 +34005,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="198" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" s="5">
         <v>359</v>
       </c>
@@ -34136,7 +34136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="199" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="5">
         <v>240</v>
       </c>
@@ -34434,7 +34434,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="201" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="5">
         <v>258</v>
       </c>
@@ -34583,7 +34583,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="202" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" s="5">
         <v>239</v>
       </c>
@@ -34750,7 +34750,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="203" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="5">
         <v>242</v>
       </c>
@@ -34917,7 +34917,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="204" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="5">
         <v>256</v>
       </c>
@@ -35084,7 +35084,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="205" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" s="5">
         <v>244</v>
       </c>
@@ -35233,7 +35233,7 @@
         <v>1952</v>
       </c>
     </row>
-    <row r="206" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="5">
         <v>285</v>
       </c>
@@ -35549,7 +35549,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="208" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="5">
         <v>237</v>
       </c>
@@ -35698,7 +35698,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="209" spans="1:43" ht="15" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:43" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" s="5">
         <v>362</v>
       </c>
@@ -40622,7 +40622,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="247" spans="1:49" ht="15" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:49" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" s="5">
         <v>363</v>
       </c>
@@ -43958,7 +43958,7 @@
         <v>1561</v>
       </c>
     </row>
-    <row r="273" spans="1:49" s="12" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:49" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A273" s="12">
         <v>463</v>
       </c>
@@ -44352,7 +44352,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="276" spans="1:49" ht="15" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:49" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" s="5">
         <v>373</v>
       </c>
@@ -44483,7 +44483,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="277" spans="1:49" ht="15" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:49" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" s="5">
         <v>369</v>
       </c>
@@ -45811,7 +45811,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="287" spans="1:49" ht="15" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:49" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" s="5">
         <v>254</v>
       </c>
@@ -47827,7 +47827,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="302" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302" s="5">
         <v>381</v>
       </c>
@@ -48745,7 +48745,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="309" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309" s="5">
         <v>383</v>
       </c>
@@ -48912,7 +48912,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="310" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310" s="5">
         <v>385</v>
       </c>
@@ -49531,7 +49531,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="315" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315" s="5">
         <v>238</v>
       </c>
@@ -49698,7 +49698,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="316" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316" s="5">
         <v>245</v>
       </c>
@@ -49865,7 +49865,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="317" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317" s="5">
         <v>255</v>
       </c>
@@ -50014,7 +50014,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="318" spans="1:55" ht="15" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:55" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318" s="5">
         <v>253</v>
       </c>
@@ -50879,10 +50879,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:BO324" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="37">
+    <filterColumn colId="25">
       <filters>
-        <filter val="产品包装"/>
-        <filter val="产品描述"/>
+        <filter val="零件数量"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -50897,15 +50896,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011C6960-2552-4A09-B632-6C090347AC28}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1959</v>
       </c>
@@ -50921,8 +50920,11 @@
       <c r="E1" t="s">
         <v>1963</v>
       </c>
+      <c r="G1" t="s">
+        <v>1959</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1960</v>
       </c>
@@ -50938,8 +50940,11 @@
       <c r="E2" t="s">
         <v>1965</v>
       </c>
+      <c r="G2" t="s">
+        <v>1608</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1961</v>
       </c>
@@ -50955,8 +50960,11 @@
       <c r="E3" t="s">
         <v>1958</v>
       </c>
+      <c r="G3" t="s">
+        <v>1965</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1964</v>
       </c>
@@ -50969,8 +50977,11 @@
       <c r="E4" t="s">
         <v>1956</v>
       </c>
+      <c r="G4" t="s">
+        <v>1964</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>1961</v>
       </c>
@@ -50980,9 +50991,36 @@
       <c r="D5" t="s">
         <v>1961</v>
       </c>
+      <c r="G5" t="s">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>1963</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G1:G9">
+    <sortCondition ref="G1:G9"/>
+  </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>